<commit_message>
Added the three methods to compute test statistics
</commit_message>
<xml_diff>
--- a/internalData/ConsistencyTestingEast.xlsx
+++ b/internalData/ConsistencyTestingEast.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajoy.mukhopadhyay\CIC\R_Packages\adaptivegmcp\internalData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DDF144-7367-4D8B-8592-C696920D9459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C700CC-ACDA-4C18-A949-C8B43C95865D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8334D68A-1C3A-4912-97B9-5ED5787DCCC6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="27">
   <si>
     <t>Design</t>
   </si>
@@ -69,12 +69,6 @@
   </si>
   <si>
     <t>FSD-2S-4EP</t>
-  </si>
-  <si>
-    <t>Nparm-Bonf</t>
-  </si>
-  <si>
-    <t>Nparm</t>
   </si>
   <si>
     <t>FSD-4S-1EP-HolmsStepDown</t>
@@ -181,7 +175,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -431,11 +425,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -450,16 +457,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -468,18 +472,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -495,10 +496,28 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -838,13 +857,13 @@
   <dimension ref="B1:J44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.54296875" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.1796875" customWidth="1"/>
@@ -854,7 +873,7 @@
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" s="20" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:9" s="14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13" t="s">
@@ -872,12 +891,12 @@
       <c r="H1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="20" t="s">
-        <v>27</v>
+      <c r="I1" s="14" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="32" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="26"/>
@@ -888,7 +907,7 @@
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B3" s="15"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="27"/>
       <c r="D3" s="3" t="s">
         <v>10</v>
@@ -905,19 +924,19 @@
       <c r="H3" s="4">
         <v>0</v>
       </c>
-      <c r="I3" s="31">
+      <c r="I3" s="17">
         <v>10000</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="33" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
+      <c r="D4" s="35" t="s">
+        <v>17</v>
       </c>
       <c r="E4" s="3">
         <v>0.66110000000000002</v>
@@ -931,16 +950,16 @@
       <c r="H4" s="4">
         <v>0</v>
       </c>
-      <c r="I4" s="31">
+      <c r="I4" s="17">
         <v>10000</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B5" s="15"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="3">
         <v>2.3800000000000002E-2</v>
       </c>
@@ -953,19 +972,19 @@
       <c r="H5" s="4">
         <v>2.3800000000000002E-2</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="17">
         <v>10000</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="33" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>12</v>
+      <c r="D6" s="35" t="s">
+        <v>16</v>
       </c>
       <c r="E6" s="3">
         <v>0.66110000000000002</v>
@@ -979,16 +998,16 @@
       <c r="H6" s="4">
         <v>0</v>
       </c>
-      <c r="I6" s="32">
+      <c r="I6" s="18">
         <v>10000</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="16"/>
+      <c r="B7" s="34"/>
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="5"/>
+      <c r="D7" s="36"/>
       <c r="E7" s="5">
         <v>2.3599999999999999E-2</v>
       </c>
@@ -1001,12 +1020,12 @@
       <c r="H7" s="6">
         <v>2.3599999999999999E-2</v>
       </c>
-      <c r="I7" s="32">
+      <c r="I7" s="18">
         <v>5000</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="32" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="1"/>
@@ -1015,15 +1034,15 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="32">
+      <c r="I8" s="18">
         <v>5000</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B9" s="15"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E9" s="3">
         <v>0.71599999999999997</v>
@@ -1037,19 +1056,19 @@
       <c r="H9" s="4">
         <v>0</v>
       </c>
-      <c r="I9" s="32">
+      <c r="I9" s="18">
         <v>10000</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="33" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>19</v>
+      <c r="D10" s="35" t="s">
+        <v>17</v>
       </c>
       <c r="E10" s="3">
         <v>0.72409999999999997</v>
@@ -1063,16 +1082,16 @@
       <c r="H10" s="4">
         <v>0</v>
       </c>
-      <c r="I10" s="32">
+      <c r="I10" s="18">
         <v>10000</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B11" s="15"/>
+      <c r="B11" s="33"/>
       <c r="C11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="27"/>
       <c r="E11" s="3">
         <v>2.2499999999999999E-2</v>
       </c>
@@ -1085,19 +1104,19 @@
       <c r="H11" s="4">
         <v>2.2499999999999999E-2</v>
       </c>
-      <c r="I11" s="32">
+      <c r="I11" s="18">
         <v>10000</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="33" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>18</v>
+      <c r="D12" s="35" t="s">
+        <v>16</v>
       </c>
       <c r="E12" s="3">
         <v>0.72</v>
@@ -1111,16 +1130,16 @@
       <c r="H12" s="4">
         <v>0</v>
       </c>
-      <c r="I12" s="32">
+      <c r="I12" s="18">
         <v>5000</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="16"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="5"/>
+      <c r="D13" s="36"/>
       <c r="E13" s="5">
         <v>1.9199999999999998E-2</v>
       </c>
@@ -1133,17 +1152,17 @@
       <c r="H13" s="6">
         <v>0.192</v>
       </c>
-      <c r="I13" s="32">
+      <c r="I13" s="18">
         <v>10000</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="31" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="28"/>
       <c r="D14" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E14" s="7">
         <v>0.73799999999999999</v>
@@ -1157,15 +1176,15 @@
       <c r="H14" s="8">
         <v>0</v>
       </c>
-      <c r="I14" s="32">
+      <c r="I14" s="18">
         <v>10000</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B15" s="18"/>
+      <c r="B15" s="21"/>
       <c r="C15" s="29"/>
       <c r="D15" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E15" s="9">
         <v>0.74399999999999999</v>
@@ -1179,19 +1198,19 @@
       <c r="H15" s="10">
         <v>0</v>
       </c>
-      <c r="I15" s="32">
+      <c r="I15" s="18">
         <v>10000</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="21" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>17</v>
+      <c r="D16" s="37" t="s">
+        <v>15</v>
       </c>
       <c r="E16" s="9">
         <v>0.73340000000000005</v>
@@ -1205,16 +1224,16 @@
       <c r="H16" s="10">
         <v>0</v>
       </c>
-      <c r="I16" s="32">
+      <c r="I16" s="18">
         <v>5000</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B17" s="18"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="9"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="9">
         <v>2.2200000000000001E-2</v>
       </c>
@@ -1227,19 +1246,19 @@
       <c r="H17" s="10">
         <v>2.2200000000000001E-2</v>
       </c>
-      <c r="I17" s="32">
+      <c r="I17" s="18">
         <v>5000</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="21" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>16</v>
+      <c r="D18" s="37" t="s">
+        <v>14</v>
       </c>
       <c r="E18" s="9">
         <v>0.73360000000000003</v>
@@ -1253,16 +1272,16 @@
       <c r="H18" s="10">
         <v>0</v>
       </c>
-      <c r="I18" s="32">
+      <c r="I18" s="18">
         <v>5000</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="19"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="11"/>
+      <c r="D19" s="38"/>
       <c r="E19" s="11">
         <v>2.2200000000000001E-2</v>
       </c>
@@ -1275,12 +1294,12 @@
       <c r="H19" s="12">
         <v>2.2200000000000001E-2</v>
       </c>
-      <c r="I19" s="32">
+      <c r="I19" s="18">
         <v>5000</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="32" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="26"/>
@@ -1291,10 +1310,10 @@
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B21" s="15"/>
+      <c r="B21" s="33"/>
       <c r="C21" s="27"/>
       <c r="D21" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E21" s="3">
         <v>0.60399999999999998</v>
@@ -1308,19 +1327,19 @@
       <c r="H21" s="4">
         <v>0</v>
       </c>
-      <c r="I21" s="31">
+      <c r="I21" s="17">
         <v>10000</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="33" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>19</v>
+      <c r="D22" s="35" t="s">
+        <v>17</v>
       </c>
       <c r="E22" s="3">
         <v>0.62419999999999998</v>
@@ -1334,16 +1353,16 @@
       <c r="H22" s="4">
         <v>0</v>
       </c>
-      <c r="I22" s="31">
+      <c r="I22" s="17">
         <v>5000</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B23" s="15"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="27"/>
       <c r="E23" s="3">
         <v>1.0200000000000001E-2</v>
       </c>
@@ -1356,19 +1375,19 @@
       <c r="H23" s="4">
         <v>1.0200000000000001E-2</v>
       </c>
-      <c r="I23" s="31">
+      <c r="I23" s="17">
         <v>5000</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="33" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>18</v>
+      <c r="D24" s="35" t="s">
+        <v>16</v>
       </c>
       <c r="E24" s="3">
         <v>0.72440000000000004</v>
@@ -1382,16 +1401,16 @@
       <c r="H24" s="4">
         <v>0</v>
       </c>
-      <c r="I24" s="31">
+      <c r="I24" s="17">
         <v>5000</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="16"/>
+      <c r="B25" s="34"/>
       <c r="C25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="5"/>
+      <c r="D25" s="36"/>
       <c r="E25" s="5">
         <v>2.0799999999999999E-2</v>
       </c>
@@ -1404,17 +1423,17 @@
       <c r="H25" s="6">
         <v>2.0799999999999999E-2</v>
       </c>
-      <c r="I25" s="31">
+      <c r="I25" s="17">
         <v>5000</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="31" t="s">
         <v>1</v>
       </c>
       <c r="C26" s="28"/>
       <c r="D26" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E26" s="7">
         <v>0.68</v>
@@ -1428,15 +1447,15 @@
       <c r="H26" s="8">
         <v>0</v>
       </c>
-      <c r="I26" s="33">
+      <c r="I26" s="19">
         <v>10000</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B27" s="18"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="29"/>
       <c r="D27" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E27" s="9">
         <v>0.73799999999999999</v>
@@ -1450,19 +1469,19 @@
       <c r="H27" s="10">
         <v>0</v>
       </c>
-      <c r="I27" s="33">
+      <c r="I27" s="19">
         <v>10000</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="21" t="s">
         <v>2</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>17</v>
+      <c r="D28" s="37" t="s">
+        <v>15</v>
       </c>
       <c r="E28" s="9">
         <v>0.69620000000000004</v>
@@ -1476,16 +1495,16 @@
       <c r="H28" s="10">
         <v>0</v>
       </c>
-      <c r="I28" s="31">
+      <c r="I28" s="17">
         <v>5000</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B29" s="18"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="9"/>
+      <c r="D29" s="29"/>
       <c r="E29" s="9">
         <v>1.7600000000000001E-2</v>
       </c>
@@ -1498,19 +1517,19 @@
       <c r="H29" s="10">
         <v>1.7600000000000001E-2</v>
       </c>
-      <c r="I29" s="31">
+      <c r="I29" s="17">
         <v>5000</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="21" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="9" t="s">
-        <v>16</v>
+      <c r="D30" s="37" t="s">
+        <v>14</v>
       </c>
       <c r="E30" s="9">
         <v>0.74119999999999997</v>
@@ -1524,16 +1543,16 @@
       <c r="H30" s="10">
         <v>0</v>
       </c>
-      <c r="I30" s="31">
+      <c r="I30" s="17">
         <v>5000</v>
       </c>
     </row>
     <row r="31" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="19"/>
+      <c r="B31" s="22"/>
       <c r="C31" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="11"/>
+      <c r="D31" s="38"/>
       <c r="E31" s="11">
         <v>2.3800000000000002E-2</v>
       </c>
@@ -1546,12 +1565,12 @@
       <c r="H31" s="12">
         <v>2.3800000000000002E-2</v>
       </c>
-      <c r="I31" s="31">
+      <c r="I31" s="17">
         <v>5000</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="32" t="s">
         <v>1</v>
       </c>
       <c r="C32" s="26"/>
@@ -1562,10 +1581,10 @@
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B33" s="15"/>
+      <c r="B33" s="33"/>
       <c r="C33" s="27"/>
       <c r="D33" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E33" s="3">
         <v>0.80400000000000005</v>
@@ -1579,19 +1598,19 @@
       <c r="H33" s="4">
         <v>0</v>
       </c>
-      <c r="I33" s="31">
+      <c r="I33" s="17">
         <v>10000</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="33" t="s">
         <v>2</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>19</v>
+      <c r="D34" s="35" t="s">
+        <v>17</v>
       </c>
       <c r="E34" s="3">
         <v>0.80620000000000003</v>
@@ -1605,16 +1624,16 @@
       <c r="H34" s="4">
         <v>0</v>
       </c>
-      <c r="I34" s="31">
+      <c r="I34" s="17">
         <v>5000</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B35" s="15"/>
+      <c r="B35" s="33"/>
       <c r="C35" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="3"/>
+      <c r="D35" s="27"/>
       <c r="E35" s="3">
         <v>0.02</v>
       </c>
@@ -1627,19 +1646,19 @@
       <c r="H35" s="4">
         <v>0.02</v>
       </c>
-      <c r="I35" s="31">
+      <c r="I35" s="17">
         <v>5000</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="33" t="s">
         <v>3</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>18</v>
+      <c r="D36" s="35" t="s">
+        <v>16</v>
       </c>
       <c r="E36" s="3">
         <v>0.8448</v>
@@ -1653,16 +1672,16 @@
       <c r="H36" s="4">
         <v>0</v>
       </c>
-      <c r="I36" s="31">
+      <c r="I36" s="17">
         <v>5000</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="16"/>
+      <c r="B37" s="34"/>
       <c r="C37" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D37" s="5"/>
+      <c r="D37" s="36"/>
       <c r="E37" s="5">
         <v>2.5399999999999999E-2</v>
       </c>
@@ -1675,7 +1694,7 @@
       <c r="H37" s="6">
         <v>2.5399999999999999E-2</v>
       </c>
-      <c r="I37" s="31">
+      <c r="I37" s="17">
         <v>5000</v>
       </c>
     </row>
@@ -1684,52 +1703,52 @@
         <v>1</v>
       </c>
       <c r="C38" s="28"/>
-      <c r="D38" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="E38" s="24">
+      <c r="D38" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" s="15">
         <v>0.84299999999999997</v>
       </c>
       <c r="F38" s="7">
         <v>0</v>
       </c>
-      <c r="G38" s="24">
+      <c r="G38" s="15">
         <v>0.84299999999999997</v>
       </c>
       <c r="H38" s="8">
         <v>0</v>
       </c>
-      <c r="I38" s="33">
+      <c r="I38" s="19">
         <v>10000</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B39" s="21"/>
+      <c r="B39" s="24"/>
       <c r="C39" s="30"/>
       <c r="D39" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E39" s="24">
+        <v>23</v>
+      </c>
+      <c r="E39" s="15">
         <v>0.68500000000000005</v>
       </c>
-      <c r="F39" s="24">
-        <v>0</v>
-      </c>
-      <c r="G39" s="24">
+      <c r="F39" s="15">
+        <v>0</v>
+      </c>
+      <c r="G39" s="15">
         <v>0.68500000000000005</v>
       </c>
-      <c r="H39" s="25">
-        <v>0</v>
-      </c>
-      <c r="I39" s="33">
+      <c r="H39" s="16">
+        <v>0</v>
+      </c>
+      <c r="I39" s="19">
         <v>10000</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B40" s="22"/>
+      <c r="B40" s="25"/>
       <c r="C40" s="29"/>
       <c r="D40" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E40" s="9">
         <v>0.83299999999999996</v>
@@ -1743,19 +1762,19 @@
       <c r="H40" s="10">
         <v>0</v>
       </c>
-      <c r="I40" s="33">
+      <c r="I40" s="19">
         <v>10000</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="21" t="s">
         <v>2</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E41" s="9">
         <v>0.84740000000000004</v>
@@ -1769,12 +1788,12 @@
       <c r="H41" s="10">
         <v>0</v>
       </c>
-      <c r="I41" s="33">
+      <c r="I41" s="19">
         <v>5000</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B42" s="18"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="9" t="s">
         <v>5</v>
       </c>
@@ -1791,19 +1810,19 @@
       <c r="H42" s="10">
         <v>2.6200000000000001E-2</v>
       </c>
-      <c r="I42" s="33">
+      <c r="I42" s="19">
         <v>5000</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="21" t="s">
         <v>3</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E43" s="9">
         <v>0.85</v>
@@ -1817,15 +1836,15 @@
       <c r="H43" s="10">
         <v>0</v>
       </c>
-      <c r="I43" s="33">
-        <v>5000</v>
-      </c>
-      <c r="J43" s="34" t="s">
-        <v>28</v>
+      <c r="I43" s="19">
+        <v>5000</v>
+      </c>
+      <c r="J43" s="20" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="19"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="11" t="s">
         <v>5</v>
       </c>
@@ -1842,13 +1861,37 @@
       <c r="H44" s="12">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="I44" s="33">
-        <v>5000</v>
-      </c>
-      <c r="J44" s="34"/>
+      <c r="I44" s="19">
+        <v>5000</v>
+      </c>
+      <c r="J44" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="40">
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
     <mergeCell ref="J43:J44"/>
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="B43:B44"/>
@@ -1865,18 +1908,6 @@
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>